<commit_message>
SyTextField: fix after audit rgaa v2 (#935)
* add SyIcon

* add prefix suffix label

* lint

* add aria-required

* add required info

* fix error message

* add helpText ptop and story

* fix label

* add error message with recommendation

* add missing autocomplete in stories

* fix tests

* fix label on prepend append slots

* fix stories

* fix ariadescribedby

* fix ariadescribedby on focus

* fix repetitive ariadescribedby value
</commit_message>
<xml_diff>
--- a/.storybook/public/audits/SyTextField.xlsx
+++ b/.storybook/public/audits/SyTextField.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/julien_roche_fabernovel_ey_com/Documents/Documents/CNAM Audits/DONE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidfyon/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCD3E6FE-9E70-415A-8596-259AA6005D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14E27E9-5BB4-1A42-8B7A-5F289A5196F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="936" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6500" yWindow="2180" windowWidth="39120" windowHeight="23560" tabRatio="936" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infos générales" sheetId="1" r:id="rId1"/>
-    <sheet name="SyTextField" sheetId="11" r:id="rId2"/>
+    <sheet name="SyTextField Audit V1" sheetId="12" r:id="rId2"/>
+    <sheet name="SyTextField Audit V2" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="303">
   <si>
     <t>Composant : SyTextField</t>
   </si>
@@ -992,12 +993,106 @@
   <si>
     <t>- https://www.accede-web.com/notices/html-et-css/formulaires/integrer-les-messages-derreur-et-les-suggestions-de-correction-directement-dans-les-balises-label/</t>
   </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>Audit V2</t>
+  </si>
+  <si>
+    <t>Certaines icônes de décoration possèdent bien le aria-hidden="true" mais le svg possède aussi le "role"="img" qui sera à retirer. C'est le cas par exemple de l'icône required.
+- Icônes valides : effacer, toutes les icônes ajoutées (prepend/append inner/outside)
+- Icônes invalides : check, warning, error</t>
+  </si>
+  <si>
+    <t>Required :
+    - Aucune indication nous informe que le champ est obligatoire dans le cas "Required" sans astérisque. Il sera préférable de forcer le cas "Required" avec cette indication de champ obligatoire =&gt; "*" dans la balise "label". Il sera à la charge du contributeur d'indiquer dans le formulaire que * = Champ obligatoire. Par ailleurs, il est recommandé d'y associer un attribut 'aria-required="true"' pour maximiser la conformité pour tout type de formulaire sur la balise input.
+- Lorsqu'un champ est en erreur, il est essentiel d'associer le message d'erreur au champ, soit dans le libellé, soit via "aria-describedby". C'était le cas lors du précédent audit mais aujourd'hui nous avons 2 problèmes :
+  - absence de "aria-describedby" reprenant l'id "input-0-messages" lorsque la div existe
+  - il y a un rôle "alert" sur la div "input-0-messages". Cela signifie que chaque champ en erreur sera restituée au lecteur d'écran en coupant la transcription orale des autres. Ce rôle en plus de l'attribut aria-live="polite" sont donc à retirer et ce sera au contributeur de gérer la gestion du focus après soumission du formulaire pour retranscrire correctement les messages d'erreur.
+- Des aides à la saisie doivent être présente et pertinente dans le cas où il y a un type de donnée ou un format spécifique à respecter avant que l'utilisateur ne commence à remplir le champ. Pour cela, il doit être présent, soit dans le libellé, soit via "aria-describedby" comme les messages d'erreurs. À la différence que le message est présent dès le début. Exemples : Validation Rules / Email (format) / Code postal (format) / Form Validation (Prénom et Âge) / Without Success Messages (format de l'email)</t>
+  </si>
+  <si>
+    <t>Chaque champ concerné par l'attribut "autocomplete" doit en posséder un. Le composant doit donc pouvoir laisser la possibilité à l'utilisateur d'utiliser ces attributs et les exemples présents dans la documentation doivent correspondrent avec ce critère.
+Par exemple :
+- Mail =&gt; autocomplete="email"
+- Tel =&gt; autocomplete="tel"
+- Prénom =&gt; autocomplete="given-name"
+- Nom =&gt; autocomplete="family-name"
+- Nom d'utilisateur =&gt; autocomplete="username"
+- Nouveau mot de passe =&gt; autocomplete="new-password"
+- Mot de passe actuel =&gt; autocomplete="current-password"
+- Code postal =&gt; autocomplete="postal-code"
+- etc.
+Pour en savoir plus : https://developer.mozilla.org/fr/docs/Web/HTML/Reference/Attributes/autocomplete
+Audit V2 : Ok pour les exemples de la documentation "Email Validation" et "Pattern Validation". Il manque les champs Nom/Prénom dans "Form Validation" et les deux champs email dans "Without Success Messages".</t>
+  </si>
+  <si>
+    <t>Aucune balise ou attribut servant à la présentation de l'information n'est présent sur le composant, les styles sont bien réalisés par CSS. 
+Une attention particulière est notée pour les espaces (sur un mot, un tableau ou pour simuler de la présentation) qui est de la responsabilité du contributeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucune erreur remontée par le validateur HTML W3C
+</t>
+  </si>
+  <si>
+    <t>Le test a été fait sur color = "primary". 
+Thème clair :
+- Libellé :
+    - normal/hover =&gt; gris 16px =&gt; 5,74 (conforme)
+        - success =&gt; vert 12px =&gt; 6,2 (conforme)
+    - focus =&gt; bleu 12 px =&gt; 9,38 (conforme)
+        - success =&gt; vert 12px =&gt; 9,56 (conforme)
+    - error (normal/hover/focus) =&gt; rouge 16/12px =&gt; 5,73 (conforme)
+- Description de l'erreur =&gt; rouge 14px =&gt; 5,73 (conforme)
+Le thème sombre ne fait pas parti de l'audit.</t>
+  </si>
+  <si>
+    <t>Le test a été fait sur color = "primary".
+Thème clair :
+- Bordure (voir texte libellé du critère 3.2 pour les success/error) :
+    - normal =&gt; non audité car possède un texte (le libellé) qui permet d'identifier la zone de saisie (voir User Interface Components &gt; Boundaries : https://www.w3.org/WAI/WCAG21/Understanding/non-text-contrast.html). En revanche, le contraste est de 2,7. Il reste recommandé d'atteindre un niveau à 3.
+    - hover =&gt; noir =&gt; 16,1 (conforme)
+    - focus =&gt; bleu =&gt; 9,38 (conforme)
+- Icône :
+    - normal =&gt; gris =&gt; 5,74 (conforme)
+    - success =&gt; vert =&gt; 3,3 (conforme)
+    - error =&gt; rouge =&gt; 5,73 (conforme)
+Le thème sombre ne fait pas parti de l'audit.</t>
+  </si>
+  <si>
+    <t>Un focus est appliqué sur l'input changeant son style. Celui est considéré comme  visible car son contraste est suffisant (voir critère 3.3).</t>
+  </si>
+  <si>
+    <t>Vicon remplacé par SyIcon</t>
+  </si>
+  <si>
+    <t>Ajout du prefix et suffix dans le label lorsqu'ils sont renseignés</t>
+  </si>
+  <si>
+    <t>Voir 11.10</t>
+  </si>
+  <si>
+    <t>Correction post audit V2 - (voir - https://github.com/assurance-maladie-digital/design-system/issues/935)</t>
+  </si>
+  <si>
+    <t>1.0.6</t>
+  </si>
+  <si>
+    <t>Ajout d'un message sur la doc pour le required
+Ajout d'aria-required lorsque required est renseigné
+Ajout d'un aria-describedby à l'input et suppression du rôle alert et de l'attribut aria-live polite
+Ajout d'une prop helpText pour l'aide à la saisie</t>
+  </si>
+  <si>
+    <t>Mise à jour des stories correspondantes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1099,7 +1194,17 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1329,7 +1434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1352,6 +1457,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1360,9 +1514,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1394,62 +1545,28 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1457,7 +1574,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1485,6 +1612,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1830,173 +1977,173 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9180BF-86F1-A847-ACFB-2DEED82D9B86}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C96" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="115.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.25" style="38" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="115.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.1" customHeight="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" ht="32" customHeight="1">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
-      <c r="A2" s="36" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" ht="19">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="34" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:6" ht="19">
+      <c r="A3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="13">
         <v>45740</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:6" ht="19" customHeight="1">
+      <c r="A4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="25" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:6" ht="16" customHeight="1">
+      <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="26">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="11">
         <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Conforme")</f>
         <v>9</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:6" ht="19" customHeight="1">
+      <c r="A6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="26">
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="11">
         <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non conforme")</f>
         <v>11</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:6" ht="19" customHeight="1">
+      <c r="A7" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="26">
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="11">
         <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non applicable")</f>
         <v>85</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="17">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:6" ht="19" customHeight="1">
+      <c r="A8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="26">
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="11">
         <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Dérogé")</f>
         <v>0</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:6" ht="19" customHeight="1">
+      <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="26">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="11">
         <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non testé")</f>
         <v>0</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:6" ht="19" customHeight="1">
+      <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="27">
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="12">
         <f>IF(SUM(D5:D6)&gt;0,D5/SUM(D5:D6),"")</f>
         <v>0.45</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:6" ht="19" customHeight="1">
+      <c r="A11" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="27">
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="12">
         <f>IF(SUM(D5:D6)&gt;0,1-ROUND(D10,2),"")</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="16">
         <v>0</v>
       </c>
     </row>
@@ -2005,7 +2152,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75">
+    <row r="13" spans="1:6" ht="20">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2018,15 +2165,15 @@
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:6" ht="34">
+      <c r="A14" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2038,11 +2185,11 @@
       <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="1:6" ht="32.25">
-      <c r="A15" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:6" ht="34">
+      <c r="A15" s="33"/>
       <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
@@ -2055,12 +2202,12 @@
       <c r="E15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30.75">
-      <c r="A16" s="15"/>
+    <row r="16" spans="1:6" ht="34">
+      <c r="A16" s="33"/>
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
@@ -2071,10 +2218,10 @@
         <v>25</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="40"/>
-    </row>
-    <row r="17" spans="1:6" ht="48">
-      <c r="A17" s="15"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="51">
+      <c r="A17" s="33"/>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2084,11 +2231,11 @@
       <c r="D17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:6" ht="32.25">
-      <c r="A18" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="1:6" ht="34">
+      <c r="A18" s="33"/>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
@@ -2098,11 +2245,11 @@
       <c r="D18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="40"/>
-    </row>
-    <row r="19" spans="1:6" ht="32.25">
-      <c r="A19" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:6" ht="34">
+      <c r="A19" s="33"/>
       <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
@@ -2112,11 +2259,11 @@
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="40"/>
-    </row>
-    <row r="20" spans="1:6" ht="32.25">
-      <c r="A20" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:6" ht="34">
+      <c r="A20" s="33"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
@@ -2126,11 +2273,11 @@
       <c r="D20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="40"/>
-    </row>
-    <row r="21" spans="1:6" ht="48">
-      <c r="A21" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="23"/>
+    </row>
+    <row r="21" spans="1:6" ht="51">
+      <c r="A21" s="33"/>
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
@@ -2140,11 +2287,11 @@
       <c r="D21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="40"/>
-    </row>
-    <row r="22" spans="1:6" ht="32.25">
-      <c r="A22" s="16"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" ht="34">
+      <c r="A22" s="34"/>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
@@ -2154,11 +2301,11 @@
       <c r="D22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="40"/>
-    </row>
-    <row r="23" spans="1:6" ht="18.75">
-      <c r="A23" s="14" t="s">
+      <c r="E22" s="15"/>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:6" ht="19">
+      <c r="A23" s="32" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2170,11 +2317,11 @@
       <c r="D23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="40"/>
-    </row>
-    <row r="24" spans="1:6" ht="32.25">
-      <c r="A24" s="16"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="1:6" ht="34">
+      <c r="A24" s="34"/>
       <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
@@ -2184,11 +2331,11 @@
       <c r="D24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="40"/>
-    </row>
-    <row r="25" spans="1:6" ht="32.25">
-      <c r="A25" s="14" t="s">
+      <c r="E24" s="15"/>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" spans="1:6" ht="34">
+      <c r="A25" s="32" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2201,10 +2348,10 @@
         <v>25</v>
       </c>
       <c r="E25" s="9"/>
-      <c r="F25" s="40"/>
-    </row>
-    <row r="26" spans="1:6" ht="292.5">
-      <c r="A26" s="15"/>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" ht="323">
+      <c r="A26" s="33"/>
       <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
@@ -2217,12 +2364,12 @@
       <c r="E26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="323.25">
-      <c r="A27" s="16"/>
+    <row r="27" spans="1:6" ht="356">
+      <c r="A27" s="34"/>
       <c r="B27" s="2" t="s">
         <v>56</v>
       </c>
@@ -2235,12 +2382,12 @@
       <c r="E27" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32.25">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:6" ht="34">
+      <c r="A28" s="32" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2252,11 +2399,11 @@
       <c r="D28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="40"/>
-    </row>
-    <row r="29" spans="1:6" ht="48">
-      <c r="A29" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:6" ht="51">
+      <c r="A29" s="33"/>
       <c r="B29" s="2" t="s">
         <v>62</v>
       </c>
@@ -2266,11 +2413,11 @@
       <c r="D29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="40"/>
-    </row>
-    <row r="30" spans="1:6" ht="32.25">
-      <c r="A30" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" spans="1:6" ht="34">
+      <c r="A30" s="33"/>
       <c r="B30" s="2" t="s">
         <v>64</v>
       </c>
@@ -2280,11 +2427,11 @@
       <c r="D30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="40"/>
-    </row>
-    <row r="31" spans="1:6" ht="32.25">
-      <c r="A31" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" spans="1:6" ht="34">
+      <c r="A31" s="33"/>
       <c r="B31" s="2" t="s">
         <v>66</v>
       </c>
@@ -2294,11 +2441,11 @@
       <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="40"/>
-    </row>
-    <row r="32" spans="1:6" ht="32.25">
-      <c r="A32" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:6" ht="34">
+      <c r="A32" s="33"/>
       <c r="B32" s="2" t="s">
         <v>68</v>
       </c>
@@ -2308,11 +2455,11 @@
       <c r="D32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="40"/>
-    </row>
-    <row r="33" spans="1:6" ht="32.25">
-      <c r="A33" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="23"/>
+    </row>
+    <row r="33" spans="1:6" ht="34">
+      <c r="A33" s="33"/>
       <c r="B33" s="2" t="s">
         <v>70</v>
       </c>
@@ -2322,11 +2469,11 @@
       <c r="D33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="40"/>
-    </row>
-    <row r="34" spans="1:6" ht="32.25">
-      <c r="A34" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="23"/>
+    </row>
+    <row r="34" spans="1:6" ht="34">
+      <c r="A34" s="33"/>
       <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
@@ -2336,11 +2483,11 @@
       <c r="D34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="40"/>
-    </row>
-    <row r="35" spans="1:6" ht="32.25">
-      <c r="A35" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="23"/>
+    </row>
+    <row r="35" spans="1:6" ht="34">
+      <c r="A35" s="33"/>
       <c r="B35" s="2" t="s">
         <v>74</v>
       </c>
@@ -2350,11 +2497,11 @@
       <c r="D35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="40"/>
-    </row>
-    <row r="36" spans="1:6" ht="32.25">
-      <c r="A36" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="23"/>
+    </row>
+    <row r="36" spans="1:6" ht="34">
+      <c r="A36" s="33"/>
       <c r="B36" s="2" t="s">
         <v>76</v>
       </c>
@@ -2364,11 +2511,11 @@
       <c r="D36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="40"/>
-    </row>
-    <row r="37" spans="1:6" ht="32.25">
-      <c r="A37" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="23"/>
+    </row>
+    <row r="37" spans="1:6" ht="34">
+      <c r="A37" s="33"/>
       <c r="B37" s="2" t="s">
         <v>78</v>
       </c>
@@ -2378,11 +2525,11 @@
       <c r="D37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="40"/>
-    </row>
-    <row r="38" spans="1:6" ht="32.25">
-      <c r="A38" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:6" ht="34">
+      <c r="A38" s="33"/>
       <c r="B38" s="2" t="s">
         <v>80</v>
       </c>
@@ -2392,11 +2539,11 @@
       <c r="D38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="40"/>
-    </row>
-    <row r="39" spans="1:6" ht="32.25">
-      <c r="A39" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="1:6" ht="34">
+      <c r="A39" s="33"/>
       <c r="B39" s="2" t="s">
         <v>82</v>
       </c>
@@ -2406,11 +2553,11 @@
       <c r="D39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="40"/>
-    </row>
-    <row r="40" spans="1:6" ht="32.25">
-      <c r="A40" s="16"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:6" ht="34">
+      <c r="A40" s="34"/>
       <c r="B40" s="2" t="s">
         <v>84</v>
       </c>
@@ -2420,11 +2567,11 @@
       <c r="D40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="31"/>
-      <c r="F40" s="40"/>
-    </row>
-    <row r="41" spans="1:6" ht="18.75">
-      <c r="A41" s="14" t="s">
+      <c r="E40" s="15"/>
+      <c r="F40" s="23"/>
+    </row>
+    <row r="41" spans="1:6" ht="19">
+      <c r="A41" s="32" t="s">
         <v>86</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2436,11 +2583,11 @@
       <c r="D41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="40"/>
-    </row>
-    <row r="42" spans="1:6" ht="32.25">
-      <c r="A42" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:6" ht="34">
+      <c r="A42" s="33"/>
       <c r="B42" s="2" t="s">
         <v>89</v>
       </c>
@@ -2450,11 +2597,11 @@
       <c r="D42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="40"/>
-    </row>
-    <row r="43" spans="1:6" ht="32.25">
-      <c r="A43" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" spans="1:6" ht="34">
+      <c r="A43" s="33"/>
       <c r="B43" s="2" t="s">
         <v>91</v>
       </c>
@@ -2464,11 +2611,11 @@
       <c r="D43" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="40"/>
-    </row>
-    <row r="44" spans="1:6" ht="32.25">
-      <c r="A44" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:6" ht="34">
+      <c r="A44" s="33"/>
       <c r="B44" s="2" t="s">
         <v>93</v>
       </c>
@@ -2478,11 +2625,11 @@
       <c r="D44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="40"/>
-    </row>
-    <row r="45" spans="1:6" ht="18.75">
-      <c r="A45" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="23"/>
+    </row>
+    <row r="45" spans="1:6" ht="19">
+      <c r="A45" s="33"/>
       <c r="B45" s="2" t="s">
         <v>95</v>
       </c>
@@ -2492,11 +2639,11 @@
       <c r="D45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="40"/>
-    </row>
-    <row r="46" spans="1:6" ht="32.25">
-      <c r="A46" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="23"/>
+    </row>
+    <row r="46" spans="1:6" ht="34">
+      <c r="A46" s="33"/>
       <c r="B46" s="2" t="s">
         <v>97</v>
       </c>
@@ -2506,11 +2653,11 @@
       <c r="D46" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="40"/>
-    </row>
-    <row r="47" spans="1:6" ht="48">
-      <c r="A47" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="23"/>
+    </row>
+    <row r="47" spans="1:6" ht="51">
+      <c r="A47" s="33"/>
       <c r="B47" s="2" t="s">
         <v>99</v>
       </c>
@@ -2520,11 +2667,11 @@
       <c r="D47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="40"/>
-    </row>
-    <row r="48" spans="1:6" ht="32.25">
-      <c r="A48" s="16"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="23"/>
+    </row>
+    <row r="48" spans="1:6" ht="34">
+      <c r="A48" s="34"/>
       <c r="B48" s="2" t="s">
         <v>101</v>
       </c>
@@ -2534,11 +2681,11 @@
       <c r="D48" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="40"/>
-    </row>
-    <row r="49" spans="1:6" ht="18.75">
-      <c r="A49" s="14" t="s">
+      <c r="E48" s="15"/>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="1:6" ht="19">
+      <c r="A49" s="32" t="s">
         <v>103</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2550,11 +2697,11 @@
       <c r="D49" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="40"/>
-    </row>
-    <row r="50" spans="1:6" ht="18.75">
-      <c r="A50" s="16"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="1:6" ht="19">
+      <c r="A50" s="34"/>
       <c r="B50" s="2" t="s">
         <v>106</v>
       </c>
@@ -2564,11 +2711,11 @@
       <c r="D50" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="40"/>
-    </row>
-    <row r="51" spans="1:6" ht="153.75">
-      <c r="A51" s="14" t="s">
+      <c r="E50" s="15"/>
+      <c r="F50" s="23"/>
+    </row>
+    <row r="51" spans="1:6" ht="170">
+      <c r="A51" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2583,12 +2730,12 @@
       <c r="E51" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F51" s="42" t="s">
+      <c r="F51" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="32.25">
-      <c r="A52" s="15"/>
+    <row r="52" spans="1:6" ht="34">
+      <c r="A52" s="33"/>
       <c r="B52" s="2" t="s">
         <v>112</v>
       </c>
@@ -2598,11 +2745,11 @@
       <c r="D52" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="40"/>
-    </row>
-    <row r="53" spans="1:6" ht="32.25">
-      <c r="A53" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="23"/>
+    </row>
+    <row r="53" spans="1:6" ht="34">
+      <c r="A53" s="33"/>
       <c r="B53" s="2" t="s">
         <v>114</v>
       </c>
@@ -2612,13 +2759,13 @@
       <c r="D53" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F53" s="40"/>
-    </row>
-    <row r="54" spans="1:6" ht="32.25">
-      <c r="A54" s="15"/>
+      <c r="F53" s="23"/>
+    </row>
+    <row r="54" spans="1:6" ht="34">
+      <c r="A54" s="33"/>
       <c r="B54" s="2" t="s">
         <v>118</v>
       </c>
@@ -2628,11 +2775,11 @@
       <c r="D54" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="31"/>
-      <c r="F54" s="40"/>
-    </row>
-    <row r="55" spans="1:6" ht="46.5">
-      <c r="A55" s="16"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="23"/>
+    </row>
+    <row r="55" spans="1:6" ht="51">
+      <c r="A55" s="34"/>
       <c r="B55" s="2" t="s">
         <v>120</v>
       </c>
@@ -2645,12 +2792,12 @@
       <c r="E55" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F55" s="42" t="s">
+      <c r="F55" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18.75">
-      <c r="A56" s="14" t="s">
+    <row r="56" spans="1:6" ht="19">
+      <c r="A56" s="32" t="s">
         <v>123</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2662,11 +2809,11 @@
       <c r="D56" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E56" s="31"/>
-      <c r="F56" s="40"/>
-    </row>
-    <row r="57" spans="1:6" ht="61.5">
-      <c r="A57" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="23"/>
+    </row>
+    <row r="57" spans="1:6" ht="68">
+      <c r="A57" s="33"/>
       <c r="B57" s="2" t="s">
         <v>126</v>
       </c>
@@ -2679,12 +2826,12 @@
       <c r="E57" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F57" s="42" t="s">
+      <c r="F57" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="18.75">
-      <c r="A58" s="15"/>
+    <row r="58" spans="1:6" ht="19">
+      <c r="A58" s="33"/>
       <c r="B58" s="2" t="s">
         <v>129</v>
       </c>
@@ -2694,11 +2841,11 @@
       <c r="D58" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E58" s="31"/>
-      <c r="F58" s="40"/>
-    </row>
-    <row r="59" spans="1:6" ht="32.25">
-      <c r="A59" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="23"/>
+    </row>
+    <row r="59" spans="1:6" ht="34">
+      <c r="A59" s="33"/>
       <c r="B59" s="2" t="s">
         <v>131</v>
       </c>
@@ -2708,11 +2855,11 @@
       <c r="D59" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E59" s="31"/>
-      <c r="F59" s="40"/>
-    </row>
-    <row r="60" spans="1:6" ht="18.75">
-      <c r="A60" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="23"/>
+    </row>
+    <row r="60" spans="1:6" ht="19">
+      <c r="A60" s="33"/>
       <c r="B60" s="2" t="s">
         <v>133</v>
       </c>
@@ -2722,11 +2869,11 @@
       <c r="D60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E60" s="31"/>
-      <c r="F60" s="40"/>
-    </row>
-    <row r="61" spans="1:6" ht="18.75">
-      <c r="A61" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="23"/>
+    </row>
+    <row r="61" spans="1:6" ht="19">
+      <c r="A61" s="33"/>
       <c r="B61" s="2" t="s">
         <v>135</v>
       </c>
@@ -2736,11 +2883,11 @@
       <c r="D61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E61" s="31"/>
-      <c r="F61" s="40"/>
-    </row>
-    <row r="62" spans="1:6" ht="32.25">
-      <c r="A62" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="23"/>
+    </row>
+    <row r="62" spans="1:6" ht="34">
+      <c r="A62" s="33"/>
       <c r="B62" s="2" t="s">
         <v>137</v>
       </c>
@@ -2750,11 +2897,11 @@
       <c r="D62" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E62" s="31"/>
-      <c r="F62" s="40"/>
-    </row>
-    <row r="63" spans="1:6" ht="32.25">
-      <c r="A63" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="23"/>
+    </row>
+    <row r="63" spans="1:6" ht="34">
+      <c r="A63" s="33"/>
       <c r="B63" s="2" t="s">
         <v>139</v>
       </c>
@@ -2764,11 +2911,11 @@
       <c r="D63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="40"/>
-    </row>
-    <row r="64" spans="1:6" ht="32.25">
-      <c r="A64" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="23"/>
+    </row>
+    <row r="64" spans="1:6" ht="34">
+      <c r="A64" s="33"/>
       <c r="B64" s="2" t="s">
         <v>141</v>
       </c>
@@ -2778,11 +2925,11 @@
       <c r="D64" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E64" s="31"/>
-      <c r="F64" s="40"/>
-    </row>
-    <row r="65" spans="1:6" ht="32.25">
-      <c r="A65" s="16"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="23"/>
+    </row>
+    <row r="65" spans="1:6" ht="34">
+      <c r="A65" s="34"/>
       <c r="B65" s="2" t="s">
         <v>143</v>
       </c>
@@ -2792,11 +2939,11 @@
       <c r="D65" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E65" s="31"/>
-      <c r="F65" s="40"/>
-    </row>
-    <row r="66" spans="1:6" ht="32.25">
-      <c r="A66" s="14" t="s">
+      <c r="E65" s="15"/>
+      <c r="F65" s="23"/>
+    </row>
+    <row r="66" spans="1:6" ht="34">
+      <c r="A66" s="32" t="s">
         <v>145</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -2808,11 +2955,11 @@
       <c r="D66" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="31"/>
-      <c r="F66" s="40"/>
-    </row>
-    <row r="67" spans="1:6" ht="32.25">
-      <c r="A67" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="23"/>
+    </row>
+    <row r="67" spans="1:6" ht="34">
+      <c r="A67" s="33"/>
       <c r="B67" s="2" t="s">
         <v>148</v>
       </c>
@@ -2822,11 +2969,11 @@
       <c r="D67" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E67" s="31"/>
-      <c r="F67" s="40"/>
-    </row>
-    <row r="68" spans="1:6" ht="18.75">
-      <c r="A68" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="23"/>
+    </row>
+    <row r="68" spans="1:6" ht="19">
+      <c r="A68" s="33"/>
       <c r="B68" s="2" t="s">
         <v>150</v>
       </c>
@@ -2836,11 +2983,11 @@
       <c r="D68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E68" s="31"/>
-      <c r="F68" s="40"/>
-    </row>
-    <row r="69" spans="1:6" ht="18.75">
-      <c r="A69" s="16"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="23"/>
+    </row>
+    <row r="69" spans="1:6" ht="34">
+      <c r="A69" s="34"/>
       <c r="B69" s="2" t="s">
         <v>152</v>
       </c>
@@ -2850,11 +2997,11 @@
       <c r="D69" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E69" s="31"/>
-      <c r="F69" s="40"/>
-    </row>
-    <row r="70" spans="1:6" ht="77.25">
-      <c r="A70" s="14" t="s">
+      <c r="E69" s="15"/>
+      <c r="F69" s="23"/>
+    </row>
+    <row r="70" spans="1:6" ht="85">
+      <c r="A70" s="32" t="s">
         <v>154</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -2869,12 +3016,12 @@
       <c r="E70" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F70" s="42" t="s">
+      <c r="F70" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="32.25">
-      <c r="A71" s="15"/>
+    <row r="71" spans="1:6" ht="34">
+      <c r="A71" s="33"/>
       <c r="B71" s="2" t="s">
         <v>158</v>
       </c>
@@ -2884,13 +3031,13 @@
       <c r="D71" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E71" s="31" t="s">
+      <c r="E71" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F71" s="40"/>
-    </row>
-    <row r="72" spans="1:6" ht="32.25">
-      <c r="A72" s="15"/>
+      <c r="F71" s="23"/>
+    </row>
+    <row r="72" spans="1:6" ht="34">
+      <c r="A72" s="33"/>
       <c r="B72" s="2" t="s">
         <v>161</v>
       </c>
@@ -2903,10 +3050,10 @@
       <c r="E72" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F72" s="40"/>
-    </row>
-    <row r="73" spans="1:6" ht="32.25">
-      <c r="A73" s="15"/>
+      <c r="F72" s="23"/>
+    </row>
+    <row r="73" spans="1:6" ht="51">
+      <c r="A73" s="33"/>
       <c r="B73" s="2" t="s">
         <v>164</v>
       </c>
@@ -2916,13 +3063,13 @@
       <c r="D73" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E73" s="31" t="s">
+      <c r="E73" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="F73" s="40"/>
-    </row>
-    <row r="74" spans="1:6" ht="32.25">
-      <c r="A74" s="15"/>
+      <c r="F73" s="23"/>
+    </row>
+    <row r="74" spans="1:6" ht="34">
+      <c r="A74" s="33"/>
       <c r="B74" s="2" t="s">
         <v>167</v>
       </c>
@@ -2935,10 +3082,10 @@
       <c r="E74" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F74" s="40"/>
-    </row>
-    <row r="75" spans="1:6" ht="32.25">
-      <c r="A75" s="15"/>
+      <c r="F74" s="23"/>
+    </row>
+    <row r="75" spans="1:6" ht="34">
+      <c r="A75" s="33"/>
       <c r="B75" s="2" t="s">
         <v>170</v>
       </c>
@@ -2948,11 +3095,11 @@
       <c r="D75" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E75" s="31"/>
-      <c r="F75" s="40"/>
-    </row>
-    <row r="76" spans="1:6" ht="32.25">
-      <c r="A76" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="23"/>
+    </row>
+    <row r="76" spans="1:6" ht="34">
+      <c r="A76" s="33"/>
       <c r="B76" s="2" t="s">
         <v>172</v>
       </c>
@@ -2965,12 +3112,12 @@
       <c r="E76" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F76" s="42" t="s">
+      <c r="F76" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="32.25">
-      <c r="A77" s="15"/>
+    <row r="77" spans="1:6" ht="34">
+      <c r="A77" s="33"/>
       <c r="B77" s="2" t="s">
         <v>175</v>
       </c>
@@ -2980,11 +3127,11 @@
       <c r="D77" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E77" s="31"/>
-      <c r="F77" s="40"/>
-    </row>
-    <row r="78" spans="1:6" ht="32.25">
-      <c r="A78" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="23"/>
+    </row>
+    <row r="78" spans="1:6" ht="51">
+      <c r="A78" s="33"/>
       <c r="B78" s="2" t="s">
         <v>177</v>
       </c>
@@ -2994,11 +3141,11 @@
       <c r="D78" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E78" s="31"/>
-      <c r="F78" s="40"/>
-    </row>
-    <row r="79" spans="1:6" ht="48">
-      <c r="A79" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="23"/>
+    </row>
+    <row r="79" spans="1:6" ht="51">
+      <c r="A79" s="33"/>
       <c r="B79" s="2" t="s">
         <v>179</v>
       </c>
@@ -3008,11 +3155,11 @@
       <c r="D79" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E79" s="31"/>
-      <c r="F79" s="40"/>
-    </row>
-    <row r="80" spans="1:6" ht="77.25">
-      <c r="A80" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="23"/>
+    </row>
+    <row r="80" spans="1:6" ht="85">
+      <c r="A80" s="33"/>
       <c r="B80" s="2" t="s">
         <v>181</v>
       </c>
@@ -3025,10 +3172,10 @@
       <c r="E80" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F80" s="40"/>
-    </row>
-    <row r="81" spans="1:6" ht="108">
-      <c r="A81" s="15"/>
+      <c r="F80" s="23"/>
+    </row>
+    <row r="81" spans="1:6" ht="119">
+      <c r="A81" s="33"/>
       <c r="B81" s="2" t="s">
         <v>184</v>
       </c>
@@ -3041,10 +3188,10 @@
       <c r="E81" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="F81" s="40"/>
-    </row>
-    <row r="82" spans="1:6" ht="48">
-      <c r="A82" s="15"/>
+      <c r="F81" s="23"/>
+    </row>
+    <row r="82" spans="1:6" ht="51">
+      <c r="A82" s="33"/>
       <c r="B82" s="2" t="s">
         <v>187</v>
       </c>
@@ -3054,11 +3201,11 @@
       <c r="D82" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E82" s="31"/>
-      <c r="F82" s="40"/>
-    </row>
-    <row r="83" spans="1:6" ht="48">
-      <c r="A83" s="16"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="23"/>
+    </row>
+    <row r="83" spans="1:6" ht="51">
+      <c r="A83" s="34"/>
       <c r="B83" s="2" t="s">
         <v>189</v>
       </c>
@@ -3068,11 +3215,11 @@
       <c r="D83" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E83" s="31"/>
-      <c r="F83" s="40"/>
-    </row>
-    <row r="84" spans="1:6" ht="18.75">
-      <c r="A84" s="14" t="s">
+      <c r="E83" s="15"/>
+      <c r="F83" s="23"/>
+    </row>
+    <row r="84" spans="1:6" ht="19">
+      <c r="A84" s="32" t="s">
         <v>191</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -3084,13 +3231,13 @@
       <c r="D84" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E84" s="31" t="s">
+      <c r="E84" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="F84" s="40"/>
-    </row>
-    <row r="85" spans="1:6" ht="32.25">
-      <c r="A85" s="15"/>
+      <c r="F84" s="23"/>
+    </row>
+    <row r="85" spans="1:6" ht="34">
+      <c r="A85" s="33"/>
       <c r="B85" s="2" t="s">
         <v>195</v>
       </c>
@@ -3100,13 +3247,13 @@
       <c r="D85" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E85" s="31" t="s">
+      <c r="E85" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="F85" s="40"/>
-    </row>
-    <row r="86" spans="1:6" ht="48">
-      <c r="A86" s="15"/>
+      <c r="F85" s="23"/>
+    </row>
+    <row r="86" spans="1:6" ht="51">
+      <c r="A86" s="33"/>
       <c r="B86" s="2" t="s">
         <v>198</v>
       </c>
@@ -3116,11 +3263,11 @@
       <c r="D86" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E86" s="31"/>
-      <c r="F86" s="40"/>
-    </row>
-    <row r="87" spans="1:6" ht="46.5">
-      <c r="A87" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="23"/>
+    </row>
+    <row r="87" spans="1:6" ht="51">
+      <c r="A87" s="33"/>
       <c r="B87" s="2" t="s">
         <v>200</v>
       </c>
@@ -3133,10 +3280,10 @@
       <c r="E87" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="F87" s="40"/>
-    </row>
-    <row r="88" spans="1:6" ht="32.25">
-      <c r="A88" s="15"/>
+      <c r="F87" s="23"/>
+    </row>
+    <row r="88" spans="1:6" ht="34">
+      <c r="A88" s="33"/>
       <c r="B88" s="2" t="s">
         <v>203</v>
       </c>
@@ -3146,11 +3293,11 @@
       <c r="D88" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E88" s="31"/>
-      <c r="F88" s="40"/>
-    </row>
-    <row r="89" spans="1:6" ht="32.25">
-      <c r="A89" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="23"/>
+    </row>
+    <row r="89" spans="1:6" ht="34">
+      <c r="A89" s="33"/>
       <c r="B89" s="2" t="s">
         <v>205</v>
       </c>
@@ -3160,11 +3307,11 @@
       <c r="D89" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E89" s="31"/>
-      <c r="F89" s="40"/>
-    </row>
-    <row r="90" spans="1:6" ht="32.25">
-      <c r="A90" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="23"/>
+    </row>
+    <row r="90" spans="1:6" ht="34">
+      <c r="A90" s="33"/>
       <c r="B90" s="2" t="s">
         <v>207</v>
       </c>
@@ -3174,11 +3321,11 @@
       <c r="D90" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E90" s="31"/>
-      <c r="F90" s="40"/>
-    </row>
-    <row r="91" spans="1:6" ht="32.25">
-      <c r="A91" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="23"/>
+    </row>
+    <row r="91" spans="1:6" ht="34">
+      <c r="A91" s="33"/>
       <c r="B91" s="2" t="s">
         <v>209</v>
       </c>
@@ -3188,11 +3335,11 @@
       <c r="D91" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E91" s="31"/>
-      <c r="F91" s="40"/>
-    </row>
-    <row r="92" spans="1:6" ht="32.25">
-      <c r="A92" s="15"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="23"/>
+    </row>
+    <row r="92" spans="1:6" ht="34">
+      <c r="A92" s="33"/>
       <c r="B92" s="2" t="s">
         <v>211</v>
       </c>
@@ -3202,11 +3349,11 @@
       <c r="D92" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="40"/>
-    </row>
-    <row r="93" spans="1:6" ht="231">
-      <c r="A93" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="23"/>
+    </row>
+    <row r="93" spans="1:6" ht="255">
+      <c r="A93" s="33"/>
       <c r="B93" s="2" t="s">
         <v>213</v>
       </c>
@@ -3219,12 +3366,12 @@
       <c r="E93" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="F93" s="43" t="s">
+      <c r="F93" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="32.25">
-      <c r="A94" s="15"/>
+    <row r="94" spans="1:6" ht="34">
+      <c r="A94" s="33"/>
       <c r="B94" s="2" t="s">
         <v>216</v>
       </c>
@@ -3237,12 +3384,12 @@
       <c r="E94" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="F94" s="44" t="s">
+      <c r="F94" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="63">
-      <c r="A95" s="15"/>
+    <row r="95" spans="1:6" ht="85">
+      <c r="A95" s="33"/>
       <c r="B95" s="2" t="s">
         <v>219</v>
       </c>
@@ -3252,11 +3399,11 @@
       <c r="D95" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E95" s="31"/>
-      <c r="F95" s="41"/>
-    </row>
-    <row r="96" spans="1:6" ht="231">
-      <c r="A96" s="16"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="24"/>
+    </row>
+    <row r="96" spans="1:6" ht="255">
+      <c r="A96" s="34"/>
       <c r="B96" s="2" t="s">
         <v>221</v>
       </c>
@@ -3269,12 +3416,12 @@
       <c r="E96" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="F96" s="42" t="s">
+      <c r="F96" s="25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="32.25">
-      <c r="A97" s="14" t="s">
+    <row r="97" spans="1:6" ht="34">
+      <c r="A97" s="32" t="s">
         <v>225</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -3286,11 +3433,11 @@
       <c r="D97" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E97" s="31"/>
-      <c r="F97" s="45"/>
-    </row>
-    <row r="98" spans="1:6" ht="32.25">
-      <c r="A98" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="23"/>
+    </row>
+    <row r="98" spans="1:6" ht="34">
+      <c r="A98" s="33"/>
       <c r="B98" s="2" t="s">
         <v>228</v>
       </c>
@@ -3300,11 +3447,11 @@
       <c r="D98" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E98" s="31"/>
-      <c r="F98" s="40"/>
-    </row>
-    <row r="99" spans="1:6" ht="18.75">
-      <c r="A99" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="23"/>
+    </row>
+    <row r="99" spans="1:6" ht="19">
+      <c r="A99" s="33"/>
       <c r="B99" s="2" t="s">
         <v>230</v>
       </c>
@@ -3314,11 +3461,11 @@
       <c r="D99" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E99" s="31"/>
-      <c r="F99" s="40"/>
-    </row>
-    <row r="100" spans="1:6" ht="32.25">
-      <c r="A100" s="15"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="23"/>
+    </row>
+    <row r="100" spans="1:6" ht="34">
+      <c r="A100" s="33"/>
       <c r="B100" s="2" t="s">
         <v>232</v>
       </c>
@@ -3328,11 +3475,11 @@
       <c r="D100" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E100" s="31"/>
-      <c r="F100" s="40"/>
-    </row>
-    <row r="101" spans="1:6" ht="32.25">
-      <c r="A101" s="15"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="23"/>
+    </row>
+    <row r="101" spans="1:6" ht="34">
+      <c r="A101" s="33"/>
       <c r="B101" s="2" t="s">
         <v>234</v>
       </c>
@@ -3342,11 +3489,11 @@
       <c r="D101" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E101" s="31"/>
-      <c r="F101" s="40"/>
-    </row>
-    <row r="102" spans="1:6" ht="63">
-      <c r="A102" s="15"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="23"/>
+    </row>
+    <row r="102" spans="1:6" ht="68">
+      <c r="A102" s="33"/>
       <c r="B102" s="2" t="s">
         <v>236</v>
       </c>
@@ -3356,11 +3503,11 @@
       <c r="D102" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E102" s="31"/>
-      <c r="F102" s="40"/>
-    </row>
-    <row r="103" spans="1:6" ht="32.25">
-      <c r="A103" s="15"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="23"/>
+    </row>
+    <row r="103" spans="1:6" ht="34">
+      <c r="A103" s="33"/>
       <c r="B103" s="2" t="s">
         <v>238</v>
       </c>
@@ -3370,11 +3517,11 @@
       <c r="D103" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E103" s="31"/>
-      <c r="F103" s="40"/>
-    </row>
-    <row r="104" spans="1:6" ht="18.75">
-      <c r="A104" s="15"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="23"/>
+    </row>
+    <row r="104" spans="1:6" ht="19">
+      <c r="A104" s="33"/>
       <c r="B104" s="2" t="s">
         <v>240</v>
       </c>
@@ -3384,11 +3531,11 @@
       <c r="D104" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E104" s="31"/>
-      <c r="F104" s="40"/>
-    </row>
-    <row r="105" spans="1:6" ht="32.25">
-      <c r="A105" s="15"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="23"/>
+    </row>
+    <row r="105" spans="1:6" ht="34">
+      <c r="A105" s="33"/>
       <c r="B105" s="2" t="s">
         <v>242</v>
       </c>
@@ -3398,13 +3545,13 @@
       <c r="D105" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E105" s="31" t="s">
+      <c r="E105" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F105" s="40"/>
-    </row>
-    <row r="106" spans="1:6" ht="48">
-      <c r="A106" s="15"/>
+      <c r="F105" s="23"/>
+    </row>
+    <row r="106" spans="1:6" ht="51">
+      <c r="A106" s="33"/>
       <c r="B106" s="2" t="s">
         <v>245</v>
       </c>
@@ -3414,11 +3561,11 @@
       <c r="D106" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E106" s="31"/>
-      <c r="F106" s="40"/>
-    </row>
-    <row r="107" spans="1:6" ht="48">
-      <c r="A107" s="16"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="23"/>
+    </row>
+    <row r="107" spans="1:6" ht="51">
+      <c r="A107" s="34"/>
       <c r="B107" s="2" t="s">
         <v>247</v>
       </c>
@@ -3428,11 +3575,11 @@
       <c r="D107" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E107" s="31"/>
-      <c r="F107" s="40"/>
-    </row>
-    <row r="108" spans="1:6" ht="32.25">
-      <c r="A108" s="14" t="s">
+      <c r="E107" s="15"/>
+      <c r="F107" s="23"/>
+    </row>
+    <row r="108" spans="1:6" ht="34">
+      <c r="A108" s="32" t="s">
         <v>249</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -3444,11 +3591,11 @@
       <c r="D108" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E108" s="31"/>
-      <c r="F108" s="40"/>
-    </row>
-    <row r="109" spans="1:6" ht="32.25">
-      <c r="A109" s="15"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="23"/>
+    </row>
+    <row r="109" spans="1:6" ht="51">
+      <c r="A109" s="33"/>
       <c r="B109" s="2" t="s">
         <v>252</v>
       </c>
@@ -3458,11 +3605,11 @@
       <c r="D109" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E109" s="31"/>
-      <c r="F109" s="40"/>
-    </row>
-    <row r="110" spans="1:6" ht="32.25">
-      <c r="A110" s="15"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="23"/>
+    </row>
+    <row r="110" spans="1:6" ht="51">
+      <c r="A110" s="33"/>
       <c r="B110" s="2" t="s">
         <v>254</v>
       </c>
@@ -3472,11 +3619,11 @@
       <c r="D110" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E110" s="31"/>
-      <c r="F110" s="40"/>
-    </row>
-    <row r="111" spans="1:6" ht="32.25">
-      <c r="A111" s="15"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="23"/>
+    </row>
+    <row r="111" spans="1:6" ht="34">
+      <c r="A111" s="33"/>
       <c r="B111" s="2" t="s">
         <v>256</v>
       </c>
@@ -3486,11 +3633,11 @@
       <c r="D111" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E111" s="31"/>
-      <c r="F111" s="40"/>
-    </row>
-    <row r="112" spans="1:6" ht="32.25">
-      <c r="A112" s="15"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="23"/>
+    </row>
+    <row r="112" spans="1:6" ht="34">
+      <c r="A112" s="33"/>
       <c r="B112" s="2" t="s">
         <v>258</v>
       </c>
@@ -3500,11 +3647,11 @@
       <c r="D112" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E112" s="31"/>
-      <c r="F112" s="40"/>
-    </row>
-    <row r="113" spans="1:6" ht="48">
-      <c r="A113" s="15"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="23"/>
+    </row>
+    <row r="113" spans="1:6" ht="51">
+      <c r="A113" s="33"/>
       <c r="B113" s="2" t="s">
         <v>260</v>
       </c>
@@ -3514,11 +3661,11 @@
       <c r="D113" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E113" s="31"/>
-      <c r="F113" s="40"/>
-    </row>
-    <row r="114" spans="1:6" ht="32.25">
-      <c r="A114" s="15"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="23"/>
+    </row>
+    <row r="114" spans="1:6" ht="34">
+      <c r="A114" s="33"/>
       <c r="B114" s="2" t="s">
         <v>262</v>
       </c>
@@ -3528,11 +3675,11 @@
       <c r="D114" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E114" s="31"/>
-      <c r="F114" s="40"/>
-    </row>
-    <row r="115" spans="1:6" ht="32.25">
-      <c r="A115" s="15"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="23"/>
+    </row>
+    <row r="115" spans="1:6" ht="34">
+      <c r="A115" s="33"/>
       <c r="B115" s="2" t="s">
         <v>264</v>
       </c>
@@ -3542,11 +3689,11 @@
       <c r="D115" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E115" s="31"/>
-      <c r="F115" s="40"/>
-    </row>
-    <row r="116" spans="1:6" ht="32.25">
-      <c r="A116" s="15"/>
+      <c r="E115" s="15"/>
+      <c r="F115" s="23"/>
+    </row>
+    <row r="116" spans="1:6" ht="34">
+      <c r="A116" s="33"/>
       <c r="B116" s="2" t="s">
         <v>266</v>
       </c>
@@ -3556,11 +3703,11 @@
       <c r="D116" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E116" s="31"/>
-      <c r="F116" s="40"/>
-    </row>
-    <row r="117" spans="1:6" ht="48">
-      <c r="A117" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="23"/>
+    </row>
+    <row r="117" spans="1:6" ht="51">
+      <c r="A117" s="33"/>
       <c r="B117" s="2" t="s">
         <v>268</v>
       </c>
@@ -3570,11 +3717,11 @@
       <c r="D117" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E117" s="31"/>
-      <c r="F117" s="40"/>
-    </row>
-    <row r="118" spans="1:6" ht="48">
-      <c r="A118" s="15"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="23"/>
+    </row>
+    <row r="118" spans="1:6" ht="51">
+      <c r="A118" s="33"/>
       <c r="B118" s="2" t="s">
         <v>270</v>
       </c>
@@ -3584,11 +3731,11 @@
       <c r="D118" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E118" s="31"/>
-      <c r="F118" s="40"/>
-    </row>
-    <row r="119" spans="1:6" ht="48">
-      <c r="A119" s="16"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="23"/>
+    </row>
+    <row r="119" spans="1:6" ht="51">
+      <c r="A119" s="34"/>
       <c r="B119" s="2" t="s">
         <v>272</v>
       </c>
@@ -3598,71 +3745,1952 @@
       <c r="D119" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E119" s="31"/>
-      <c r="F119" s="40"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="23"/>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="24" t="s">
+      <c r="A122" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="B122" s="24"/>
-      <c r="C122" s="24"/>
-      <c r="D122" s="24"/>
+      <c r="B122" s="28"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="28"/>
       <c r="E122" s="7" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="51.95" customHeight="1">
-      <c r="A123" s="10" t="s">
+    <row r="123" spans="1:6" ht="52" customHeight="1">
+      <c r="A123" s="29" t="s">
         <v>276</v>
       </c>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="12"/>
+      <c r="B123" s="30"/>
+      <c r="C123" s="30"/>
+      <c r="D123" s="31"/>
       <c r="E123" s="8" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="30.75">
-      <c r="A124" s="10" t="s">
+    <row r="124" spans="1:6" ht="34">
+      <c r="A124" s="29" t="s">
         <v>278</v>
       </c>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="12"/>
+      <c r="B124" s="30"/>
+      <c r="C124" s="30"/>
+      <c r="D124" s="31"/>
       <c r="E124" s="8" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="36.950000000000003" customHeight="1">
-      <c r="A125" s="10" t="s">
+    <row r="125" spans="1:6" ht="37" customHeight="1">
+      <c r="A125" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="12"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="30"/>
+      <c r="D125" s="31"/>
       <c r="E125" s="8" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="75" customHeight="1">
-      <c r="A126" s="10" t="s">
+      <c r="A126" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="12"/>
+      <c r="B126" s="30"/>
+      <c r="C126" s="30"/>
+      <c r="D126" s="31"/>
       <c r="E126" s="8" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="101.1" customHeight="1">
-      <c r="A127" s="10" t="s">
+    <row r="127" spans="1:6" ht="101" customHeight="1">
+      <c r="A127" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="30"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="31"/>
+      <c r="E127" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A40"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A56:A65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A83"/>
+    <mergeCell ref="A84:A96"/>
+    <mergeCell ref="A97:A107"/>
+    <mergeCell ref="A108:A119"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A126:D126"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D14:E119">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$D14="Non testé"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$D14="Conforme"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$D14="Non conforme"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D119" xr:uid="{3385A7A8-3AC5-7046-B4F0-1B31CE5500C7}">
+      <formula1>"Conforme,Non conforme,Non applicable,Dérogé,Non testé"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format JJ/MM/AAAA" sqref="D3" xr:uid="{A3ACFD28-EFB7-434F-AE94-7E240239510B}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="115.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32" customHeight="1">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" ht="19">
+      <c r="A2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19">
+      <c r="A3" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="13">
+        <v>45863</v>
+      </c>
+      <c r="E3" s="47">
+        <v>45876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19" customHeight="1">
+      <c r="A4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1">
+      <c r="A5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Conforme")</f>
+        <v>14</v>
+      </c>
+      <c r="E5" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19" customHeight="1">
+      <c r="A6" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non conforme")</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19" customHeight="1">
+      <c r="A7" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non applicable")</f>
+        <v>85</v>
+      </c>
+      <c r="E7" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non applicable")</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19" customHeight="1">
+      <c r="A8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Dérogé")</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Dérogé")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19" customHeight="1">
+      <c r="A9" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non testé")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <f xml:space="preserve"> COUNTIF($D$13:$D$118,"Non testé")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19" customHeight="1">
+      <c r="A10" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="12">
+        <f>IF(SUM(D5:D6)&gt;0,D5/SUM(D5:D6),"")</f>
+        <v>0.7</v>
+      </c>
+      <c r="E10" s="12">
+        <f>IF(SUM(E5:E6)&gt;0,E5/SUM(E5:E6),"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19" customHeight="1">
+      <c r="A11" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="12">
+        <f>IF(SUM(D5:D6)&gt;0,1-ROUND(D10,2),"")</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E11" s="12">
+        <f>IF(SUM(E5:E6)&gt;0,1-ROUND(E10,2),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="20">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="34">
+      <c r="A14" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:6" ht="85">
+      <c r="A15" s="33"/>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="34">
+      <c r="A16" s="33"/>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="51">
+      <c r="A17" s="33"/>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="1:6" ht="34">
+      <c r="A18" s="33"/>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:6" ht="34">
+      <c r="A19" s="33"/>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:6" ht="34">
+      <c r="A20" s="33"/>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="23"/>
+    </row>
+    <row r="21" spans="1:6" ht="51">
+      <c r="A21" s="33"/>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" ht="34">
+      <c r="A22" s="34"/>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:6" ht="19">
+      <c r="A23" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="1:6" ht="34">
+      <c r="A24" s="34"/>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" spans="1:6" ht="34">
+      <c r="A25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" ht="204">
+      <c r="A26" s="33"/>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F26" s="23"/>
+    </row>
+    <row r="27" spans="1:6" ht="255">
+      <c r="A27" s="34"/>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="F27" s="23"/>
+    </row>
+    <row r="28" spans="1:6" ht="34">
+      <c r="A28" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:6" ht="51">
+      <c r="A29" s="33"/>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" spans="1:6" ht="34">
+      <c r="A30" s="33"/>
+      <c r="B30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" spans="1:6" ht="34">
+      <c r="A31" s="33"/>
+      <c r="B31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="15"/>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:6" ht="34">
+      <c r="A32" s="33"/>
+      <c r="B32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="23"/>
+    </row>
+    <row r="33" spans="1:6" ht="34">
+      <c r="A33" s="33"/>
+      <c r="B33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="23"/>
+    </row>
+    <row r="34" spans="1:6" ht="34">
+      <c r="A34" s="33"/>
+      <c r="B34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="23"/>
+    </row>
+    <row r="35" spans="1:6" ht="34">
+      <c r="A35" s="33"/>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="23"/>
+    </row>
+    <row r="36" spans="1:6" ht="34">
+      <c r="A36" s="33"/>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="23"/>
+    </row>
+    <row r="37" spans="1:6" ht="34">
+      <c r="A37" s="33"/>
+      <c r="B37" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:6" ht="34">
+      <c r="A38" s="33"/>
+      <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="1:6" ht="34">
+      <c r="A39" s="33"/>
+      <c r="B39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:6" ht="34">
+      <c r="A40" s="34"/>
+      <c r="B40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="23"/>
+    </row>
+    <row r="41" spans="1:6" ht="19">
+      <c r="A41" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:6" ht="34">
+      <c r="A42" s="33"/>
+      <c r="B42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" spans="1:6" ht="34">
+      <c r="A43" s="33"/>
+      <c r="B43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:6" ht="34">
+      <c r="A44" s="33"/>
+      <c r="B44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="23"/>
+    </row>
+    <row r="45" spans="1:6" ht="34">
+      <c r="A45" s="33"/>
+      <c r="B45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="23"/>
+    </row>
+    <row r="46" spans="1:6" ht="34">
+      <c r="A46" s="33"/>
+      <c r="B46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="23"/>
+    </row>
+    <row r="47" spans="1:6" ht="51">
+      <c r="A47" s="33"/>
+      <c r="B47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="23"/>
+    </row>
+    <row r="48" spans="1:6" ht="34">
+      <c r="A48" s="34"/>
+      <c r="B48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="1:6" ht="19">
+      <c r="A49" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="1:6" ht="19">
+      <c r="A50" s="34"/>
+      <c r="B50" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="23"/>
+    </row>
+    <row r="51" spans="1:6" ht="170">
+      <c r="A51" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F51" s="45" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="34">
+      <c r="A52" s="33"/>
+      <c r="B52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="15"/>
+      <c r="F52" s="23"/>
+    </row>
+    <row r="53" spans="1:6" ht="34">
+      <c r="A53" s="33"/>
+      <c r="B53" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" s="23"/>
+    </row>
+    <row r="54" spans="1:6" ht="34">
+      <c r="A54" s="33"/>
+      <c r="B54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="15"/>
+      <c r="F54" s="23"/>
+    </row>
+    <row r="55" spans="1:6" ht="51">
+      <c r="A55" s="34"/>
+      <c r="B55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F55" s="45" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="19">
+      <c r="A56" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" s="15"/>
+      <c r="F56" s="23"/>
+    </row>
+    <row r="57" spans="1:6" ht="34">
+      <c r="A57" s="33"/>
+      <c r="B57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="F57" s="23"/>
+    </row>
+    <row r="58" spans="1:6" ht="19">
+      <c r="A58" s="33"/>
+      <c r="B58" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="15"/>
+      <c r="F58" s="23"/>
+    </row>
+    <row r="59" spans="1:6" ht="34">
+      <c r="A59" s="33"/>
+      <c r="B59" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="15"/>
+      <c r="F59" s="23"/>
+    </row>
+    <row r="60" spans="1:6" ht="19">
+      <c r="A60" s="33"/>
+      <c r="B60" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="23"/>
+    </row>
+    <row r="61" spans="1:6" ht="19">
+      <c r="A61" s="33"/>
+      <c r="B61" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="15"/>
+      <c r="F61" s="23"/>
+    </row>
+    <row r="62" spans="1:6" ht="34">
+      <c r="A62" s="33"/>
+      <c r="B62" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="15"/>
+      <c r="F62" s="23"/>
+    </row>
+    <row r="63" spans="1:6" ht="34">
+      <c r="A63" s="33"/>
+      <c r="B63" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="15"/>
+      <c r="F63" s="23"/>
+    </row>
+    <row r="64" spans="1:6" ht="34">
+      <c r="A64" s="33"/>
+      <c r="B64" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" s="15"/>
+      <c r="F64" s="23"/>
+    </row>
+    <row r="65" spans="1:6" ht="34">
+      <c r="A65" s="34"/>
+      <c r="B65" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="15"/>
+      <c r="F65" s="23"/>
+    </row>
+    <row r="66" spans="1:6" ht="34">
+      <c r="A66" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="23"/>
+    </row>
+    <row r="67" spans="1:6" ht="34">
+      <c r="A67" s="33"/>
+      <c r="B67" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" s="15"/>
+      <c r="F67" s="23"/>
+    </row>
+    <row r="68" spans="1:6" ht="19">
+      <c r="A68" s="33"/>
+      <c r="B68" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" s="15"/>
+      <c r="F68" s="23"/>
+    </row>
+    <row r="69" spans="1:6" ht="34">
+      <c r="A69" s="34"/>
+      <c r="B69" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="15"/>
+      <c r="F69" s="23"/>
+    </row>
+    <row r="70" spans="1:6" ht="51">
+      <c r="A70" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="F70" s="23"/>
+    </row>
+    <row r="71" spans="1:6" ht="34">
+      <c r="A71" s="33"/>
+      <c r="B71" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F71" s="23"/>
+    </row>
+    <row r="72" spans="1:6" ht="34">
+      <c r="A72" s="33"/>
+      <c r="B72" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F72" s="23"/>
+    </row>
+    <row r="73" spans="1:6" ht="51">
+      <c r="A73" s="33"/>
+      <c r="B73" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F73" s="23"/>
+    </row>
+    <row r="74" spans="1:6" ht="34">
+      <c r="A74" s="33"/>
+      <c r="B74" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F74" s="23"/>
+    </row>
+    <row r="75" spans="1:6" ht="34">
+      <c r="A75" s="33"/>
+      <c r="B75" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E75" s="15"/>
+      <c r="F75" s="23"/>
+    </row>
+    <row r="76" spans="1:6" ht="34">
+      <c r="A76" s="33"/>
+      <c r="B76" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="F76" s="23"/>
+    </row>
+    <row r="77" spans="1:6" ht="34">
+      <c r="A77" s="33"/>
+      <c r="B77" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E77" s="15"/>
+      <c r="F77" s="23"/>
+    </row>
+    <row r="78" spans="1:6" ht="51">
+      <c r="A78" s="33"/>
+      <c r="B78" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E78" s="15"/>
+      <c r="F78" s="23"/>
+    </row>
+    <row r="79" spans="1:6" ht="51">
+      <c r="A79" s="33"/>
+      <c r="B79" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" s="15"/>
+      <c r="F79" s="23"/>
+    </row>
+    <row r="80" spans="1:6" ht="85">
+      <c r="A80" s="33"/>
+      <c r="B80" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F80" s="23"/>
+    </row>
+    <row r="81" spans="1:6" ht="119">
+      <c r="A81" s="33"/>
+      <c r="B81" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F81" s="23"/>
+    </row>
+    <row r="82" spans="1:6" ht="51">
+      <c r="A82" s="33"/>
+      <c r="B82" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E82" s="15"/>
+      <c r="F82" s="23"/>
+    </row>
+    <row r="83" spans="1:6" ht="51">
+      <c r="A83" s="34"/>
+      <c r="B83" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E83" s="15"/>
+      <c r="F83" s="23"/>
+    </row>
+    <row r="84" spans="1:6" ht="19">
+      <c r="A84" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="F84" s="23"/>
+    </row>
+    <row r="85" spans="1:6" ht="34">
+      <c r="A85" s="33"/>
+      <c r="B85" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F85" s="23"/>
+    </row>
+    <row r="86" spans="1:6" ht="51">
+      <c r="A86" s="33"/>
+      <c r="B86" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E86" s="15"/>
+      <c r="F86" s="23"/>
+    </row>
+    <row r="87" spans="1:6" ht="51">
+      <c r="A87" s="33"/>
+      <c r="B87" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F87" s="23"/>
+    </row>
+    <row r="88" spans="1:6" ht="34">
+      <c r="A88" s="33"/>
+      <c r="B88" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E88" s="15"/>
+      <c r="F88" s="23"/>
+    </row>
+    <row r="89" spans="1:6" ht="34">
+      <c r="A89" s="33"/>
+      <c r="B89" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E89" s="15"/>
+      <c r="F89" s="23"/>
+    </row>
+    <row r="90" spans="1:6" ht="34">
+      <c r="A90" s="33"/>
+      <c r="B90" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E90" s="15"/>
+      <c r="F90" s="23"/>
+    </row>
+    <row r="91" spans="1:6" ht="34">
+      <c r="A91" s="33"/>
+      <c r="B91" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E91" s="15"/>
+      <c r="F91" s="23"/>
+    </row>
+    <row r="92" spans="1:6" ht="34">
+      <c r="A92" s="33"/>
+      <c r="B92" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E92" s="15"/>
+      <c r="F92" s="23"/>
+    </row>
+    <row r="93" spans="1:6" ht="289">
+      <c r="A93" s="33"/>
+      <c r="B93" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F93" s="46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="34">
+      <c r="A94" s="33"/>
+      <c r="B94" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="F94" s="48" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="85">
+      <c r="A95" s="33"/>
+      <c r="B95" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E95" s="15"/>
+      <c r="F95" s="24"/>
+    </row>
+    <row r="96" spans="1:6" ht="306">
+      <c r="A96" s="34"/>
+      <c r="B96" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F96" s="49" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="34">
+      <c r="A97" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E97" s="15"/>
+      <c r="F97" s="23"/>
+    </row>
+    <row r="98" spans="1:6" ht="34">
+      <c r="A98" s="33"/>
+      <c r="B98" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E98" s="15"/>
+      <c r="F98" s="23"/>
+    </row>
+    <row r="99" spans="1:6" ht="19">
+      <c r="A99" s="33"/>
+      <c r="B99" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E99" s="15"/>
+      <c r="F99" s="23"/>
+    </row>
+    <row r="100" spans="1:6" ht="34">
+      <c r="A100" s="33"/>
+      <c r="B100" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" s="15"/>
+      <c r="F100" s="23"/>
+    </row>
+    <row r="101" spans="1:6" ht="34">
+      <c r="A101" s="33"/>
+      <c r="B101" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E101" s="15"/>
+      <c r="F101" s="23"/>
+    </row>
+    <row r="102" spans="1:6" ht="68">
+      <c r="A102" s="33"/>
+      <c r="B102" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E102" s="15"/>
+      <c r="F102" s="23"/>
+    </row>
+    <row r="103" spans="1:6" ht="34">
+      <c r="A103" s="33"/>
+      <c r="B103" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E103" s="15"/>
+      <c r="F103" s="23"/>
+    </row>
+    <row r="104" spans="1:6" ht="19">
+      <c r="A104" s="33"/>
+      <c r="B104" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E104" s="15"/>
+      <c r="F104" s="23"/>
+    </row>
+    <row r="105" spans="1:6" ht="34">
+      <c r="A105" s="33"/>
+      <c r="B105" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E105" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F105" s="23"/>
+    </row>
+    <row r="106" spans="1:6" ht="51">
+      <c r="A106" s="33"/>
+      <c r="B106" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E106" s="15"/>
+      <c r="F106" s="23"/>
+    </row>
+    <row r="107" spans="1:6" ht="51">
+      <c r="A107" s="34"/>
+      <c r="B107" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E107" s="15"/>
+      <c r="F107" s="23"/>
+    </row>
+    <row r="108" spans="1:6" ht="34">
+      <c r="A108" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E108" s="15"/>
+      <c r="F108" s="23"/>
+    </row>
+    <row r="109" spans="1:6" ht="51">
+      <c r="A109" s="33"/>
+      <c r="B109" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E109" s="15"/>
+      <c r="F109" s="23"/>
+    </row>
+    <row r="110" spans="1:6" ht="51">
+      <c r="A110" s="33"/>
+      <c r="B110" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E110" s="15"/>
+      <c r="F110" s="23"/>
+    </row>
+    <row r="111" spans="1:6" ht="34">
+      <c r="A111" s="33"/>
+      <c r="B111" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E111" s="15"/>
+      <c r="F111" s="23"/>
+    </row>
+    <row r="112" spans="1:6" ht="34">
+      <c r="A112" s="33"/>
+      <c r="B112" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E112" s="15"/>
+      <c r="F112" s="23"/>
+    </row>
+    <row r="113" spans="1:6" ht="51">
+      <c r="A113" s="33"/>
+      <c r="B113" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E113" s="15"/>
+      <c r="F113" s="23"/>
+    </row>
+    <row r="114" spans="1:6" ht="34">
+      <c r="A114" s="33"/>
+      <c r="B114" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E114" s="15"/>
+      <c r="F114" s="23"/>
+    </row>
+    <row r="115" spans="1:6" ht="34">
+      <c r="A115" s="33"/>
+      <c r="B115" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E115" s="15"/>
+      <c r="F115" s="23"/>
+    </row>
+    <row r="116" spans="1:6" ht="51">
+      <c r="A116" s="33"/>
+      <c r="B116" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E116" s="15"/>
+      <c r="F116" s="23"/>
+    </row>
+    <row r="117" spans="1:6" ht="51">
+      <c r="A117" s="33"/>
+      <c r="B117" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E117" s="15"/>
+      <c r="F117" s="23"/>
+    </row>
+    <row r="118" spans="1:6" ht="51">
+      <c r="A118" s="33"/>
+      <c r="B118" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E118" s="15"/>
+      <c r="F118" s="23"/>
+    </row>
+    <row r="119" spans="1:6" ht="51">
+      <c r="A119" s="34"/>
+      <c r="B119" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E119" s="15"/>
+      <c r="F119" s="23"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="B122" s="28"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="52" customHeight="1">
+      <c r="A123" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="B123" s="30"/>
+      <c r="C123" s="30"/>
+      <c r="D123" s="31"/>
+      <c r="E123" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="34">
+      <c r="A124" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="B124" s="30"/>
+      <c r="C124" s="30"/>
+      <c r="D124" s="31"/>
+      <c r="E124" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="37" customHeight="1">
+      <c r="A125" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="B125" s="30"/>
+      <c r="C125" s="30"/>
+      <c r="D125" s="31"/>
+      <c r="E125" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="75" customHeight="1">
+      <c r="A126" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="B126" s="30"/>
+      <c r="C126" s="30"/>
+      <c r="D126" s="31"/>
+      <c r="E126" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="101" customHeight="1">
+      <c r="A127" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="B127" s="30"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="31"/>
       <c r="E127" s="8" t="s">
         <v>285</v>
       </c>
@@ -3701,18 +5729,14 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:E119">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$D14="Non conforme"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:E119">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$D14="Non testé"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:E119">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$D14="Conforme"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>$D14="Non conforme"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>